<commit_message>
Added remittance and returning classes for Santander
</commit_message>
<xml_diff>
--- a/docs/Santander CNAB 400.xlsx
+++ b/docs/Santander CNAB 400.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Remessa" sheetId="1" state="visible" r:id="rId2"/>
@@ -133,7 +133,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Conta movimento velha (8 posições): preencher com o conjunto de números informados pelo Banco (SCCM). Conta movimento nova (9 posições): preencher com as 8 primeiras posições da </t>
+      <t xml:space="preserve">Conta movimento velha (8 posições): preencher com o conjunto de números informados pelo Banco (SCCM). Conta movimento nova (10 posições): preencher com as 8 primeiras posições da </t>
     </r>
     <r>
       <rPr>
@@ -826,7 +826,7 @@
     <t>228 a 240</t>
   </si>
   <si>
-    <t>Valor do abatimento concedido </t>
+    <t>Valor do abatimento concedido</t>
   </si>
   <si>
     <t>241 a 253</t>
@@ -1271,8 +1271,8 @@
   </sheetPr>
   <dimension ref="A1:V84"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C72" activeCellId="0" sqref="C72"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1599,7 +1599,7 @@
       <c r="U10" s="7"/>
       <c r="V10" s="7"/>
     </row>
-    <row r="11" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>36</v>
       </c>
@@ -2311,7 +2311,7 @@
       <c r="U33" s="7"/>
       <c r="V33" s="7"/>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
         <v>89</v>
       </c>
@@ -2341,7 +2341,7 @@
       <c r="U34" s="7"/>
       <c r="V34" s="7"/>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
         <v>92</v>
       </c>
@@ -2587,7 +2587,7 @@
       <c r="U42" s="7"/>
       <c r="V42" s="7"/>
     </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="7" t="s">
         <v>115</v>
       </c>
@@ -2619,7 +2619,7 @@
       <c r="U43" s="7"/>
       <c r="V43" s="7"/>
     </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="7" t="s">
         <v>118</v>
       </c>
@@ -2651,7 +2651,7 @@
       <c r="U44" s="7"/>
       <c r="V44" s="7"/>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="7" t="s">
         <v>121</v>
       </c>
@@ -2805,7 +2805,7 @@
       <c r="U49" s="7"/>
       <c r="V49" s="7"/>
     </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="7" t="s">
         <v>134</v>
       </c>
@@ -2837,7 +2837,7 @@
       <c r="U50" s="7"/>
       <c r="V50" s="7"/>
     </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="7" t="s">
         <v>138</v>
       </c>
@@ -2931,7 +2931,7 @@
       <c r="U53" s="7"/>
       <c r="V53" s="7"/>
     </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="7" t="s">
         <v>146</v>
       </c>
@@ -2963,7 +2963,7 @@
       <c r="U54" s="7"/>
       <c r="V54" s="7"/>
     </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="7" t="s">
         <v>149</v>
       </c>
@@ -2995,7 +2995,7 @@
       <c r="U55" s="7"/>
       <c r="V55" s="7"/>
     </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="7" t="s">
         <v>151</v>
       </c>
@@ -3025,7 +3025,7 @@
       <c r="U56" s="7"/>
       <c r="V56" s="7"/>
     </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="7" t="s">
         <v>153</v>
       </c>
@@ -3085,7 +3085,7 @@
       <c r="U58" s="7"/>
       <c r="V58" s="7"/>
     </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="7" t="s">
         <v>158</v>
       </c>
@@ -3541,7 +3541,7 @@
       <c r="U73" s="7"/>
       <c r="V73" s="7"/>
     </row>
-    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="7" t="s">
         <v>193</v>
       </c>
@@ -3603,7 +3603,7 @@
       <c r="U75" s="7"/>
       <c r="V75" s="7"/>
     </row>
-    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="7" t="s">
         <v>72</v>
       </c>
@@ -3755,7 +3755,7 @@
       <c r="U80" s="7"/>
       <c r="V80" s="7"/>
     </row>
-    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="7" t="s">
         <v>199</v>
       </c>
@@ -3845,7 +3845,7 @@
       <c r="U83" s="7"/>
       <c r="V83" s="7"/>
     </row>
-    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="7" t="s">
         <v>72</v>
       </c>
@@ -3893,8 +3893,8 @@
   </sheetPr>
   <dimension ref="A1:V98"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A89" activeCellId="0" sqref="A89"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>